<commit_message>
sort transactions by date
</commit_message>
<xml_diff>
--- a/xl.xlsx
+++ b/xl.xlsx
@@ -18,6 +18,12 @@
     <sheet name="123213 ( 7979 )" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="aDSFH ( 56873 )" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="VBCZ ( 87112 )" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Date_test ( 29 )" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="test2 ( 2112 )" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="test_last ( 213522 )" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="last ( 1111111 )" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="my_last ( 9999 )" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="loop ( 777 )" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -571,8 +577,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -631,7 +635,6 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>1</v>
       </c>
@@ -651,6 +654,286 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>VBCZ</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>87112</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>التاريخ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>الخدمه</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>التكلفه</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>المدفوع</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>الرصيد</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>الملاحظات</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>مسلسل</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>13/01/2000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب مرتبات</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date_test</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>29</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>التاريخ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>الخدمه</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>التكلفه</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>المدفوع</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>الرصيد</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>الملاحظات</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>مسلسل</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>بطاقه ضريبيه</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>90</v>
+      </c>
+      <c r="E4" t="n">
+        <v>90</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب مرتبات</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="n">
+        <v>80</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -667,11 +950,11 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>VBCZ</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>87112</v>
+        <v>2112</v>
       </c>
       <c r="C1" t="n">
         <v>1</v>
@@ -681,8 +964,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -724,35 +1005,1072 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>90</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test_last</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>213522</v>
+      </c>
+      <c r="C1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>التاريخ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>الخدمه</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>التكلفه</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>المدفوع</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>الرصيد</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>الملاحظات</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>مسلسل</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>اضافة سياره</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1600</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E5" t="n">
+        <v>700</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>44574</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10/01/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب قيمه مضافه</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="n">
+        <v>11500</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11/01/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11500</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>11/01/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="n">
+        <v>11500</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>last</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1111111</v>
+      </c>
+      <c r="C1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>التاريخ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>الخدمه</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>التكلفه</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>المدفوع</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>الرصيد</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>الملاحظات</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>مسلسل</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب قيمه مضافه</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>17/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اضافة سياره</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>900</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>17/01/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>اضافة سياره</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>900</v>
+      </c>
+      <c r="D7" t="n">
+        <v>200</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2600</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2609</v>
+      </c>
+      <c r="G9" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>my_last</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>9999</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>التاريخ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>الخدمه</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>التكلفه</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>المدفوع</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>الرصيد</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>الملاحظات</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>مسلسل</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" t="n">
+        <v>900</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب مرتبات</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>900</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>loop</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>777</v>
+      </c>
+      <c r="C1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>التاريخ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>الخدمه</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>التكلفه</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>المدفوع</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>الرصيد</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>الملاحظات</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>مسلسل</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>05/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>بطاقه ضريبيه</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>44566</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>44568</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10/01/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>90</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>10</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>44571</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>10/01/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>90</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>10</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>44571</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>11/01/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب قيمه مضافه</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>90</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>44572</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>11/01/2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>11</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>44572</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>12/01/2022</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>200</v>
+      </c>
+      <c r="D10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>44573</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب قيمه مضافه</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>90</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>13</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>44574</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>14/01/2022</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>اقرار ضرائب مرتبات</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2022</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>12</v>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>90</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>14</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>44575</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05/01/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>تجديد اشتراك البوابه الالكترونيه</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>90</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>5</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>44931</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +2084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P1048577"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -1002,6 +2320,105 @@
       </c>
       <c r="P8" t="n">
         <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>12/01/2020</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2020</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>12/01/2022</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب عامه</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1048577">
+      <c r="A1048577" t="inlineStr">
+        <is>
+          <t>04/01/2022</t>
+        </is>
+      </c>
+      <c r="B1048577" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C1048577" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1048577" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1048577" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G1048577" t="n">
+        <v>7</v>
+      </c>
+      <c r="H1048577" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I1048577" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1048577" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1010,6 +2427,236 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Client 2</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>التاريخ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>الخدمه</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>التكلفه</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>المدفوع</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>الرصيد</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>الملاحظات</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>مسلسل</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>تسوية ملف ضريبى</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>comment .......</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>12/01/2022</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>100</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>شسي</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>اتعاب لجنه داخلية</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>اضافة سياره</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>اقرار ضرائب مرتبات</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>200</v>
+      </c>
+      <c r="D9" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1026,11 +2673,11 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Client 2</t>
+          <t>amr ahmad mahmoud al</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
         <v>1</v>
@@ -1081,22 +2728,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>تسوية ملف ضريبى</t>
+          <t>اقرار ضرائب عامه</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>comment .......</t>
-        </is>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -1114,16 +2756,11 @@
     <row r="5">
       <c r="K5" t="inlineStr">
         <is>
-          <t>12/01/2022</t>
+          <t>13/01/2022</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>100</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>شسي</t>
-        </is>
+        <v>1110</v>
       </c>
       <c r="N5" t="n">
         <v>2022</v>
@@ -1132,109 +2769,7 @@
         <v>1</v>
       </c>
       <c r="P5" t="n">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>amr ahmad mahmoud al</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>التاريخ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>الخدمه</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>التكلفه</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>المدفوع</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>الرصيد</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>الملاحظات</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>مسلسل</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>07/01/2022</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>اقرار ضرائب عامه</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2022</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1248,7 +2783,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1266,7 +2801,7 @@
         <v>111</v>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="n">
         <v>21</v>
@@ -1355,6 +2890,39 @@
       </c>
       <c r="J4" t="n">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1368,7 +2936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1386,7 +2954,7 @@
         <v>213</v>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="inlineStr">
         <is>
@@ -1444,39 +3012,114 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>04/01/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>اعداد و مراجعة ميزانيه</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>44565</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>11/01/2022</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>اعداد و مراجعة ميزانيه</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>123</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>123</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>يسب</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2022</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
         <v>11</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>44572</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>13/01/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>تجديد اشتراك البوابه الالكترونيه</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>13</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>44574</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +3133,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1591,6 +3234,54 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12/01/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>200</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>telephone</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12/01/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>telephone(dec)</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>